<commit_message>
working on formatting of data
</commit_message>
<xml_diff>
--- a/data/ModelF_Herceptin_Params.xlsx
+++ b/data/ModelF_Herceptin_Params.xlsx
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="157">
   <si>
     <t>Parameter</t>
   </si>
@@ -348,12 +348,6 @@
     <t>Tumo-&gt;Central Transit</t>
   </si>
   <si>
-    <t>Drug or Sol Complex</t>
-  </si>
-  <si>
-    <t>Sol Target</t>
-  </si>
-  <si>
     <t>Molecular Weight</t>
   </si>
   <si>
@@ -504,16 +498,46 @@
     <t>check ~ 0.3 or ~1</t>
   </si>
   <si>
-    <t>Formula from Sameed's analysis .</t>
-  </si>
-  <si>
-    <t>chosen so that back and forth rates are equal</t>
-  </si>
-  <si>
     <t>Marked guess because there are differing views if B = 0.3 (Deng16) or 1 (Thurber12)</t>
   </si>
   <si>
     <t>Not used in model, but you should check to make sure it's around 0.3-1, otherwise parameters are odd</t>
+  </si>
+  <si>
+    <t>Permeability</t>
+  </si>
+  <si>
+    <t>Capillary Radius</t>
+  </si>
+  <si>
+    <t>Krogh Cylindar Radius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Void fraction </t>
+  </si>
+  <si>
+    <t>Central--&gt;Tumor Transit : Thurber</t>
+  </si>
+  <si>
+    <t>Central--&gt;Tumor Transit : Proportional</t>
+  </si>
+  <si>
+    <t>Tumor--&gt;Central Transit : Thurber</t>
+  </si>
+  <si>
+    <t>Tumor--&gt;Central Transit : Proportional</t>
+  </si>
+  <si>
+    <t>Tumor-&gt;Central Transit</t>
+  </si>
+  <si>
+    <t>Drug or Sol</t>
+  </si>
+  <si>
+    <t>chosen so that back and forth rates are equal (Thurber12)</t>
+  </si>
+  <si>
+    <t>Formula from Sameed's analysis with 3 from B = 1/3</t>
   </si>
 </sst>
 </file>
@@ -710,7 +734,37 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -1112,21 +1166,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J65" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J65" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:J65"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Order" dataDxfId="11"/>
-    <tableColumn id="2" name="ParamType" dataDxfId="10"/>
-    <tableColumn id="3" name="Molecule" dataDxfId="9"/>
-    <tableColumn id="4" name="Description" dataDxfId="8"/>
-    <tableColumn id="5" name="Parameter" dataDxfId="7"/>
-    <tableColumn id="6" name="Value" dataDxfId="6"/>
-    <tableColumn id="7" name="Units" dataDxfId="5"/>
-    <tableColumn id="8" name="Source" dataDxfId="4"/>
-    <tableColumn id="10" name="Formula" dataDxfId="3">
+    <tableColumn id="1" name="Order" dataDxfId="14"/>
+    <tableColumn id="2" name="ParamType" dataDxfId="13"/>
+    <tableColumn id="3" name="Molecule" dataDxfId="12"/>
+    <tableColumn id="4" name="Description" dataDxfId="11"/>
+    <tableColumn id="5" name="Parameter" dataDxfId="10"/>
+    <tableColumn id="6" name="Value" dataDxfId="9"/>
+    <tableColumn id="7" name="Units" dataDxfId="8"/>
+    <tableColumn id="8" name="Source" dataDxfId="7"/>
+    <tableColumn id="10" name="Formula" dataDxfId="6">
       <calculatedColumnFormula>_xlfn.IFNA(_xlfn.FORMULATEXT(F2),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Comment or Reference" dataDxfId="2"/>
+    <tableColumn id="9" name="Comment or Reference" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1456,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1498,10 +1552,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>43</v>
@@ -1530,7 +1584,7 @@
         <v>3</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I2" s="15" t="str">
         <f t="shared" ref="I2:I33" ca="1" si="0">_xlfn.IFNA(_xlfn.FORMULATEXT(F2),"")</f>
@@ -1561,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I3" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1599,7 +1653,7 @@
         <v/>
       </c>
       <c r="J4" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1664,7 +1718,7 @@
         <v/>
       </c>
       <c r="J6" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1697,7 +1751,7 @@
         <v/>
       </c>
       <c r="J7" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1730,7 +1784,7 @@
         <v/>
       </c>
       <c r="J8" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1811,7 +1865,7 @@
         <v>67</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F11" s="3">
         <f>VD1_</f>
@@ -1843,7 +1897,7 @@
         <v>68</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F12" s="3">
         <f>VD1_</f>
@@ -1923,10 +1977,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>=Q/VD2_</v>
       </c>
-      <c r="J14" s="9" t="str">
-        <f t="shared" ref="J14" ca="1" si="1">_xlfn.FORMULATEXT(F14)</f>
-        <v>=Q/VD2_</v>
-      </c>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
@@ -1939,16 +1990,16 @@
         <v>71</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F15" s="3">
         <v>145</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>55</v>
@@ -1958,7 +2009,7 @@
         <v/>
       </c>
       <c r="J15" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -1972,16 +2023,16 @@
         <v>81</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F16" s="3">
         <v>68.599999999999994</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>55</v>
@@ -1991,7 +2042,7 @@
         <v/>
       </c>
       <c r="J16" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -2005,17 +2056,17 @@
         <v>73</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F17" s="3">
         <f>MWS</f>
         <v>68.599999999999994</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>55</v>
@@ -2025,7 +2076,7 @@
         <v>=MWS</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -2058,7 +2109,7 @@
         <v/>
       </c>
       <c r="J18" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -2091,7 +2142,7 @@
         <v/>
       </c>
       <c r="J19" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2124,7 +2175,7 @@
         <v/>
       </c>
       <c r="J20" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2157,7 +2208,7 @@
         <v/>
       </c>
       <c r="J21" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2190,7 +2241,7 @@
         <v/>
       </c>
       <c r="J22" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -2216,14 +2267,14 @@
         <v>4</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I23" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="J23" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2249,7 +2300,7 @@
         <v>4</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I24" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2280,14 +2331,14 @@
         <v>19</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I25" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="J25" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2313,29 +2364,31 @@
         <v>19</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I26" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
       <c r="J26" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>20.100000000000001</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="C27" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F27" s="12">
         <v>830</v>
@@ -2351,7 +2404,7 @@
         <v/>
       </c>
       <c r="J27" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -2409,7 +2462,7 @@
         <v>4</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I29" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2440,7 +2493,7 @@
         <v>4</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I30" s="15" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -2456,7 +2509,7 @@
         <v>49</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>85</v>
@@ -2511,10 +2564,7 @@
         <f t="shared" ca="1" si="0"/>
         <v>=VD3_</v>
       </c>
-      <c r="J32" s="9" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(VtumS)</f>
-        <v>=VD3_</v>
-      </c>
+      <c r="J32" s="9"/>
     </row>
     <row r="33" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="8">
@@ -2546,14 +2596,15 @@
         <f t="shared" ca="1" si="0"/>
         <v>=VD3_</v>
       </c>
-      <c r="J33" s="9" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(VtumS)</f>
-        <v>=VD3_</v>
-      </c>
+      <c r="J33" s="9"/>
     </row>
     <row r="34" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
+      <c r="A34" s="8">
+        <v>26.1</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="C34" s="8" t="s">
         <v>81</v>
       </c>
@@ -2561,7 +2612,7 @@
         <v>85</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F34" s="3">
         <f>VD3_</f>
@@ -2574,17 +2625,18 @@
         <v>54</v>
       </c>
       <c r="I34" s="15" t="str">
-        <f t="shared" ref="I34:I65" ca="1" si="2">_xlfn.IFNA(_xlfn.FORMULATEXT(F34),"")</f>
+        <f t="shared" ref="I34:I65" ca="1" si="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F34),"")</f>
         <v>=VD3_</v>
       </c>
-      <c r="J34" s="9" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(VtumS)</f>
-        <v>=VD3_</v>
-      </c>
+      <c r="J34" s="9"/>
     </row>
     <row r="35" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
+      <c r="A35" s="8">
+        <v>26.2</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="C35" s="8" t="s">
         <v>84</v>
       </c>
@@ -2592,7 +2644,7 @@
         <v>85</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F35" s="3">
         <f>VD3_</f>
@@ -2605,13 +2657,10 @@
         <v>54</v>
       </c>
       <c r="I35" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>=VD3_</v>
       </c>
-      <c r="J35" s="9" t="str">
-        <f ca="1">_xlfn.FORMULATEXT(VtumS)</f>
-        <v>=VD3_</v>
-      </c>
+      <c r="J35" s="9"/>
     </row>
     <row r="36" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
@@ -2636,14 +2685,14 @@
         <v>4</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I36" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J36" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2669,14 +2718,14 @@
         <v>4</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I37" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J37" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2702,14 +2751,14 @@
         <v>4</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I38" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J38" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2738,11 +2787,11 @@
         <v>55</v>
       </c>
       <c r="I39" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J39" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -2771,11 +2820,11 @@
         <v>55</v>
       </c>
       <c r="I40" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J40" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -2786,13 +2835,13 @@
         <v>49</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F41" s="17">
         <f>k13D*(Vc/Vtum)/(keD3_+k31D)</f>
@@ -2802,14 +2851,14 @@
         <v>3</v>
       </c>
       <c r="H41" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I41" s="21" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=k13D*(Vc/Vtum)/(keD3_+k31D)</v>
+      </c>
+      <c r="J41" s="22" t="s">
         <v>144</v>
-      </c>
-      <c r="I41" s="21" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>=k13D*(Vc/Vtum)/(keD3_+k31D)</v>
-      </c>
-      <c r="J41" s="22" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -2820,13 +2869,13 @@
         <v>49</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F42" s="3">
         <v>0</v>
@@ -2835,97 +2884,129 @@
         <v>3</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I42" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J42" s="9"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
+      <c r="A43" s="8">
+        <v>33.1</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>145</v>
+      </c>
       <c r="E43" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F43" s="3">
         <f>0.000000003*1000000*60*60*24</f>
         <v>259.2</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>55</v>
       </c>
       <c r="I43" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>=0.000000003*1000000*60*60*24</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
+      <c r="A44" s="8">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>146</v>
+      </c>
       <c r="E44" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F44" s="3">
         <v>8</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>55</v>
       </c>
       <c r="I44" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J44" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
+      <c r="A45" s="8">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>147</v>
+      </c>
       <c r="E45" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F45" s="3">
         <v>75</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>55</v>
       </c>
       <c r="I45" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J45" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
+      <c r="A46" s="8">
+        <v>33.4</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>148</v>
+      </c>
       <c r="E46" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F46" s="3">
         <v>1</v>
@@ -2934,23 +3015,31 @@
         <v>3</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I46" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J46" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
+      <c r="A47" s="8">
+        <v>33.5</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>149</v>
+      </c>
       <c r="E47" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F47" s="3">
         <f>k31D_thurber*VD3_/VD1_</f>
@@ -2963,20 +3052,28 @@
         <v>54</v>
       </c>
       <c r="I47" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>=k31D_thurber*VD3_/VD1_</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
+      <c r="A48" s="8">
+        <v>33.6</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>150</v>
+      </c>
       <c r="E48" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F48" s="3">
         <f>k12D*VD3_/VD2_</f>
@@ -2989,7 +3086,7 @@
         <v>54</v>
       </c>
       <c r="I48" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>=k12D*VD3_/VD2_</v>
       </c>
       <c r="J48" s="9"/>
@@ -3021,11 +3118,11 @@
         <v>57</v>
       </c>
       <c r="I49" s="14" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>=k13d_prop</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3051,14 +3148,14 @@
         <v>4</v>
       </c>
       <c r="H50" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I50" s="15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="J50" s="9" t="s">
         <v>128</v>
-      </c>
-      <c r="I50" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="J50" s="9" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3084,10 +3181,10 @@
         <v>4</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I51" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J51" s="9" t="s">
@@ -3095,12 +3192,20 @@
       </c>
     </row>
     <row r="52" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
+      <c r="A52" s="8">
+        <v>36.1</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>151</v>
+      </c>
       <c r="E52" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F52" s="3">
         <f>2*P*Rcap/Rkrogh^2</f>
@@ -3113,20 +3218,28 @@
         <v>54</v>
       </c>
       <c r="I52" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>=2*P*Rcap/Rkrogh^2</v>
       </c>
       <c r="J52" s="16" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
+      <c r="A53" s="8">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>152</v>
+      </c>
       <c r="E53" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F53" s="3">
         <f>VD1_/VD3_*k13d_prop*3</f>
@@ -3139,11 +3252,11 @@
         <v>54</v>
       </c>
       <c r="I53" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v>=VD1_/VD3_*k13d_prop*3</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3157,7 +3270,7 @@
         <v>71</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>12</v>
@@ -3172,12 +3285,12 @@
       <c r="H54" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="I54" s="19" t="str">
-        <f t="shared" ca="1" si="2"/>
+      <c r="I54" s="20" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>=k31D_prop</v>
       </c>
       <c r="J54" s="20" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3191,7 +3304,7 @@
         <v>73</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="E55" s="2" t="s">
         <v>29</v>
@@ -3203,14 +3316,14 @@
         <v>4</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I55" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J55" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3224,7 +3337,7 @@
         <v>74</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>92</v>
+        <v>153</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>31</v>
@@ -3236,14 +3349,14 @@
         <v>4</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I56" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J56" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -3260,7 +3373,7 @@
         <v>80</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F57" s="3">
         <v>0</v>
@@ -3269,10 +3382,10 @@
         <v>19</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I57" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J57" s="13"/>
@@ -3288,10 +3401,10 @@
         <v>81</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F58" s="3">
         <v>0</v>
@@ -3300,10 +3413,10 @@
         <v>4</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I58" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J58" s="9"/>
@@ -3319,10 +3432,10 @@
         <v>84</v>
       </c>
       <c r="D59" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="F59" s="3">
         <v>0</v>
@@ -3331,10 +3444,10 @@
         <v>4</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I59" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J59" s="9"/>
@@ -3347,13 +3460,13 @@
         <v>50</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>89</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F60" s="3">
         <v>1</v>
@@ -3362,10 +3475,10 @@
         <v>4</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I60" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J60" s="9"/>
@@ -3378,13 +3491,13 @@
         <v>50</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>90</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F61" s="3">
         <v>1</v>
@@ -3393,10 +3506,10 @@
         <v>4</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I61" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J61" s="9"/>
@@ -3415,7 +3528,7 @@
         <v>91</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F62" s="3">
         <v>0</v>
@@ -3424,10 +3537,10 @@
         <v>4</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I62" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J62" s="9"/>
@@ -3446,7 +3559,7 @@
         <v>92</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F63" s="3">
         <v>0</v>
@@ -3455,10 +3568,10 @@
         <v>4</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I63" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J63" s="10"/>
@@ -3471,13 +3584,13 @@
         <v>49</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>91</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F64" s="3">
         <v>0</v>
@@ -3486,10 +3599,10 @@
         <v>4</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I64" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J64" s="9"/>
@@ -3502,13 +3615,13 @@
         <v>49</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>92</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F65" s="3">
         <v>0</v>
@@ -3517,52 +3630,52 @@
         <v>4</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I65" s="15" t="str">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
       <c r="J65" s="9"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F280">
-    <cfRule type="containsText" dxfId="23" priority="11" operator="containsText" text="derived">
+    <cfRule type="containsText" dxfId="26" priority="11" operator="containsText" text="derived">
       <formula>NOT(ISERROR(SEARCH("derived",F280)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="expression" dxfId="22" priority="9">
+    <cfRule type="expression" dxfId="25" priority="9">
       <formula>$H2="fit"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A23:G28 J23:K28 A43:C45 A46:D46 H43:I46 K43:K46 I3:I65 A29:K42 A1:K22 A47:K1048576">
-    <cfRule type="containsText" dxfId="21" priority="8" operator="containsText" text="calc">
+  <conditionalFormatting sqref="A23:G28 J23:K28 H43:I46 K43:K46 I3:I65 A1:K22 A54:K1048576 C47:K53 D46 A29:K42 A43:B53 C43:C46">
+    <cfRule type="containsText" dxfId="24" priority="8" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I22 H29:I1048576 I3:I65">
-    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="23" priority="6" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="22" priority="7" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H1:I1048576">
-    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="not used">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="not used">
       <formula>NOT(ISERROR(SEARCH("not used",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="5" operator="containsText" text="check">
+    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="check">
       <formula>NOT(ISERROR(SEARCH("check",H1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixing bug in ODE, now use VM1, VDM1, VM3, VDM3 instead of VD1 and VD3
</commit_message>
<xml_diff>
--- a/data/ModelF_Herceptin_Params.xlsx
+++ b/data/ModelF_Herceptin_Params.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28702"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="500" yWindow="2160" windowWidth="26960" windowHeight="16280" tabRatio="500"/>
+    <workbookView xWindow="7480" yWindow="2580" windowWidth="26960" windowHeight="16280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1461,8 +1461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>